<commit_message>
Update Copia de 2019-02-28_Training sample pour l'ordonnancement_Cellule Robotisée_Rev1 (6).xlsx
</commit_message>
<xml_diff>
--- a/Copia de 2019-02-28_Training sample pour l'ordonnancement_Cellule Robotisée_Rev1 (6).xlsx
+++ b/Copia de 2019-02-28_Training sample pour l'ordonnancement_Cellule Robotisée_Rev1 (6).xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abigail\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abigail\Documents\GitHub\datos_pasantia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0225BB6-0E6A-45D4-AFAF-7F8BBEEECF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EADD65-4FE8-4DE3-B889-091122D54AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="données" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">données!$A$1:$L$78</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -24,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t># pièce</t>
   </si>
@@ -114,12 +115,6 @@
   </si>
   <si>
     <t>40815</t>
-  </si>
-  <si>
-    <t>19816</t>
-  </si>
-  <si>
-    <t>92317</t>
   </si>
   <si>
     <t>61318</t>
@@ -609,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L998"/>
+  <dimension ref="A1:L996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -678,23 +673,23 @@
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="10">
-        <f t="shared" ref="H2:H80" si="0">B2+C2</f>
+        <f t="shared" ref="H2:H78" si="0">B2+C2</f>
         <v>6.3179550000000004</v>
       </c>
       <c r="I2" s="7">
-        <f t="shared" ref="I2:I80" si="1">IF(AND(NOT(ISBLANK(F2)),NOT(ISBLANK(G2))),2,1)</f>
+        <f t="shared" ref="I2:I78" si="1">IF(AND(NOT(ISBLANK(F2)),NOT(ISBLANK(G2))),2,1)</f>
         <v>1</v>
       </c>
       <c r="J2" s="7">
-        <f t="shared" ref="J2:J80" si="2">IF(ISBLANK(D2),0,1)</f>
+        <f t="shared" ref="J2:J78" si="2">IF(ISBLANK(D2),0,1)</f>
         <v>0</v>
       </c>
       <c r="K2" s="7">
-        <f t="shared" ref="K2:K80" si="3">IF(ISBLANK(G2),F2,G2)</f>
+        <f t="shared" ref="K2:K78" si="3">IF(ISBLANK(G2),F2,G2)</f>
         <v>1</v>
       </c>
       <c r="L2" s="7">
-        <f t="shared" ref="L2:L80" si="4">IF(ISBLANK(G2),2,F2)</f>
+        <f t="shared" ref="L2:L78" si="4">IF(ISBLANK(G2),2,F2)</f>
         <v>2</v>
       </c>
     </row>
@@ -1201,27 +1196,23 @@
         <v>26</v>
       </c>
       <c r="B17" s="3">
-        <v>5.1623000000000001</v>
-      </c>
-      <c r="C17" s="3">
-        <v>3.1675</v>
-      </c>
+        <v>33.323399999999999</v>
+      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="2">
         <v>1</v>
       </c>
       <c r="F17" s="2">
-        <v>2</v>
-      </c>
-      <c r="G17" s="2">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G17" s="2"/>
       <c r="H17" s="4">
         <f t="shared" si="0"/>
-        <v>8.3298000000000005</v>
+        <v>33.323399999999999</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="2"/>
@@ -1240,11 +1231,9 @@
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="3">
-        <v>5.1623000000000001</v>
-      </c>
+      <c r="B18" s="3"/>
       <c r="C18" s="3">
-        <v>3.1675</v>
+        <v>9.2915700000000001</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
@@ -1252,16 +1241,14 @@
       <c r="F18" s="2">
         <v>2</v>
       </c>
-      <c r="G18" s="2">
-        <v>1</v>
-      </c>
+      <c r="G18" s="2"/>
       <c r="H18" s="4">
         <f t="shared" si="0"/>
-        <v>8.3298000000000005</v>
+        <v>9.2915700000000001</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="2"/>
@@ -1269,31 +1256,31 @@
       </c>
       <c r="K18" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="3">
-        <v>33.323399999999999</v>
-      </c>
-      <c r="C19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3">
+        <v>8.1133500000000005</v>
+      </c>
       <c r="D19" s="2">
         <v>1</v>
       </c>
       <c r="F19" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="4">
         <f t="shared" si="0"/>
-        <v>33.323399999999999</v>
+        <v>8.1133500000000005</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="1"/>
@@ -1305,31 +1292,31 @@
       </c>
       <c r="K19" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3">
-        <v>9.2915700000000001</v>
-      </c>
+      <c r="B20" s="3">
+        <v>8.2979000000000003</v>
+      </c>
+      <c r="C20" s="3"/>
       <c r="D20" s="2">
         <v>1</v>
       </c>
       <c r="F20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="4">
         <f t="shared" si="0"/>
-        <v>9.2915700000000001</v>
+        <v>8.2979000000000003</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="1"/>
@@ -1341,7 +1328,7 @@
       </c>
       <c r="K20" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" si="4"/>
@@ -1354,7 +1341,7 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3">
-        <v>8.1133500000000005</v>
+        <v>3.3992800000000001</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -1365,7 +1352,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="4">
         <f t="shared" si="0"/>
-        <v>8.1133500000000005</v>
+        <v>3.3992800000000001</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="1"/>
@@ -1424,9 +1411,11 @@
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="3">
+        <v>8.32</v>
+      </c>
       <c r="C23" s="3">
-        <v>3.3992800000000001</v>
+        <v>8.599219999999999</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
@@ -1434,14 +1423,16 @@
       <c r="F23" s="2">
         <v>2</v>
       </c>
-      <c r="G23" s="2"/>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
       <c r="H23" s="4">
         <f t="shared" si="0"/>
-        <v>3.3992800000000001</v>
+        <v>16.919219999999999</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="2"/>
@@ -1449,7 +1440,7 @@
       </c>
       <c r="K23" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="4"/>
@@ -1460,20 +1451,20 @@
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="3">
-        <v>8.2979000000000003</v>
-      </c>
-      <c r="C24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
+        <v>5.21835</v>
+      </c>
       <c r="D24" s="2">
         <v>1</v>
       </c>
       <c r="F24" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="4">
         <f t="shared" si="0"/>
-        <v>8.2979000000000003</v>
+        <v>5.21835</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="1"/>
@@ -1485,7 +1476,7 @@
       </c>
       <c r="K24" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" si="4"/>
@@ -1496,11 +1487,9 @@
       <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="3">
-        <v>8.32</v>
-      </c>
+      <c r="B25" s="3"/>
       <c r="C25" s="3">
-        <v>8.599219999999999</v>
+        <v>8.1133500000000005</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
@@ -1508,16 +1497,14 @@
       <c r="F25" s="2">
         <v>2</v>
       </c>
-      <c r="G25" s="2">
-        <v>1</v>
-      </c>
+      <c r="G25" s="2"/>
       <c r="H25" s="4">
         <f t="shared" si="0"/>
-        <v>16.919219999999999</v>
+        <v>8.1133500000000005</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="2"/>
@@ -1525,7 +1512,7 @@
       </c>
       <c r="K25" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" si="4"/>
@@ -1536,20 +1523,20 @@
       <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3">
-        <v>5.21835</v>
-      </c>
+      <c r="B26" s="3">
+        <v>33.323399999999999</v>
+      </c>
+      <c r="C26" s="3"/>
       <c r="D26" s="2">
         <v>1</v>
       </c>
       <c r="F26" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="4">
         <f t="shared" si="0"/>
-        <v>5.21835</v>
+        <v>33.323399999999999</v>
       </c>
       <c r="I26" s="1">
         <f t="shared" si="1"/>
@@ -1561,7 +1548,7 @@
       </c>
       <c r="K26" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L26" s="1">
         <f t="shared" si="4"/>
@@ -1574,7 +1561,7 @@
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3">
-        <v>8.1133500000000005</v>
+        <v>3.3992800000000001</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
@@ -1585,7 +1572,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="4">
         <f t="shared" si="0"/>
-        <v>8.1133500000000005</v>
+        <v>3.3992800000000001</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" si="1"/>
@@ -1609,19 +1596,17 @@
         <v>37</v>
       </c>
       <c r="B28" s="3">
-        <v>33.323399999999999</v>
+        <v>3.4674999999999998</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="2">
-        <v>1</v>
-      </c>
+      <c r="D28" s="2"/>
       <c r="F28" s="2">
         <v>1</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="4">
         <f t="shared" si="0"/>
-        <v>33.323399999999999</v>
+        <v>3.4674999999999998</v>
       </c>
       <c r="I28" s="1">
         <f t="shared" si="1"/>
@@ -1629,7 +1614,7 @@
       </c>
       <c r="J28" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" s="1">
         <f t="shared" si="3"/>
@@ -1646,18 +1631,16 @@
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3">
-        <v>3.3992800000000001</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
+        <v>2.7459750000000001</v>
+      </c>
+      <c r="D29" s="2"/>
       <c r="F29" s="2">
         <v>2</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="4">
         <f t="shared" si="0"/>
-        <v>3.3992800000000001</v>
+        <v>2.7459750000000001</v>
       </c>
       <c r="I29" s="1">
         <f t="shared" si="1"/>
@@ -1665,7 +1648,7 @@
       </c>
       <c r="J29" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29" s="1">
         <f t="shared" si="3"/>
@@ -1680,18 +1663,20 @@
       <c r="A30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="3">
-        <v>3.4674999999999998</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3">
+        <v>5.7393899999999993</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
       <c r="F30" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="4">
         <f t="shared" si="0"/>
-        <v>3.4674999999999998</v>
+        <v>5.7393899999999993</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" si="1"/>
@@ -1699,11 +1684,11 @@
       </c>
       <c r="J30" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" si="4"/>
@@ -1716,7 +1701,7 @@
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3">
-        <v>2.7459750000000001</v>
+        <v>2.9125000000000001</v>
       </c>
       <c r="D31" s="2"/>
       <c r="F31" s="2">
@@ -1725,7 +1710,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="4">
         <f t="shared" si="0"/>
-        <v>2.7459750000000001</v>
+        <v>2.9125000000000001</v>
       </c>
       <c r="I31" s="1">
         <f t="shared" si="1"/>
@@ -1750,18 +1735,16 @@
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3">
-        <v>5.7393899999999993</v>
-      </c>
-      <c r="D32" s="2">
-        <v>1</v>
-      </c>
+        <v>2.7459750000000001</v>
+      </c>
+      <c r="D32" s="2"/>
       <c r="F32" s="2">
         <v>2</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="4">
         <f t="shared" si="0"/>
-        <v>5.7393899999999993</v>
+        <v>2.7459750000000001</v>
       </c>
       <c r="I32" s="1">
         <f t="shared" si="1"/>
@@ -1769,7 +1752,7 @@
       </c>
       <c r="J32" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" s="1">
         <f t="shared" si="3"/>
@@ -1788,7 +1771,9 @@
       <c r="C33" s="3">
         <v>2.9125000000000001</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
       <c r="F33" s="2">
         <v>2</v>
       </c>
@@ -1803,7 +1788,7 @@
       </c>
       <c r="J33" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" s="1">
         <f t="shared" si="3"/>
@@ -1820,7 +1805,7 @@
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3">
-        <v>2.7459750000000001</v>
+        <v>6.6361999999999997</v>
       </c>
       <c r="D34" s="2"/>
       <c r="F34" s="2">
@@ -1829,7 +1814,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="4">
         <f t="shared" si="0"/>
-        <v>2.7459750000000001</v>
+        <v>6.6361999999999997</v>
       </c>
       <c r="I34" s="1">
         <f t="shared" si="1"/>
@@ -1854,7 +1839,7 @@
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3">
-        <v>2.9125000000000001</v>
+        <v>7.7179000000000002</v>
       </c>
       <c r="D35" s="2">
         <v>1</v>
@@ -1865,7 +1850,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="4">
         <f t="shared" si="0"/>
-        <v>2.9125000000000001</v>
+        <v>7.7179000000000002</v>
       </c>
       <c r="I35" s="1">
         <f t="shared" si="1"/>
@@ -1890,16 +1875,18 @@
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3">
-        <v>6.6361999999999997</v>
-      </c>
-      <c r="D36" s="2"/>
+        <v>6.8976499999999996</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
       <c r="F36" s="2">
         <v>2</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="4">
         <f t="shared" si="0"/>
-        <v>6.6361999999999997</v>
+        <v>6.8976499999999996</v>
       </c>
       <c r="I36" s="1">
         <f t="shared" si="1"/>
@@ -1907,7 +1894,7 @@
       </c>
       <c r="J36" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="1">
         <f t="shared" si="3"/>
@@ -1960,18 +1947,16 @@
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3">
-        <v>6.8976499999999996</v>
-      </c>
-      <c r="D38" s="2">
-        <v>1</v>
-      </c>
+        <v>6.6361999999999997</v>
+      </c>
+      <c r="D38" s="2"/>
       <c r="F38" s="2">
         <v>2</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="4">
         <f t="shared" si="0"/>
-        <v>6.8976499999999996</v>
+        <v>6.6361999999999997</v>
       </c>
       <c r="I38" s="1">
         <f t="shared" si="1"/>
@@ -1979,7 +1964,7 @@
       </c>
       <c r="J38" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38" s="1">
         <f t="shared" si="3"/>
@@ -1996,7 +1981,7 @@
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3">
-        <v>7.7179000000000002</v>
+        <v>9.6173500000000001</v>
       </c>
       <c r="D39" s="2">
         <v>1</v>
@@ -2007,7 +1992,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="4">
         <f t="shared" si="0"/>
-        <v>7.7179000000000002</v>
+        <v>9.6173500000000001</v>
       </c>
       <c r="I39" s="1">
         <f t="shared" si="1"/>
@@ -2032,16 +2017,18 @@
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3">
-        <v>6.6361999999999997</v>
-      </c>
-      <c r="D40" s="2"/>
+        <v>9.6173500000000001</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
+      </c>
       <c r="F40" s="2">
         <v>2</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="4">
         <f t="shared" si="0"/>
-        <v>6.6361999999999997</v>
+        <v>9.6173500000000001</v>
       </c>
       <c r="I40" s="1">
         <f t="shared" si="1"/>
@@ -2049,7 +2036,7 @@
       </c>
       <c r="J40" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" s="1">
         <f t="shared" si="3"/>
@@ -2066,7 +2053,7 @@
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3">
-        <v>9.6173500000000001</v>
+        <v>6.8976499999999996</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -2077,7 +2064,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="4">
         <f t="shared" si="0"/>
-        <v>9.6173500000000001</v>
+        <v>6.8976499999999996</v>
       </c>
       <c r="I41" s="1">
         <f t="shared" si="1"/>
@@ -2100,9 +2087,11 @@
       <c r="A42" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="3"/>
+      <c r="B42" s="3">
+        <v>19.733854999999998</v>
+      </c>
       <c r="C42" s="3">
-        <v>9.6173500000000001</v>
+        <v>8.9113800000000012</v>
       </c>
       <c r="D42" s="2">
         <v>1</v>
@@ -2110,14 +2099,16 @@
       <c r="F42" s="2">
         <v>2</v>
       </c>
-      <c r="G42" s="2"/>
+      <c r="G42" s="2">
+        <v>1</v>
+      </c>
       <c r="H42" s="4">
         <f t="shared" si="0"/>
-        <v>9.6173500000000001</v>
+        <v>28.645235</v>
       </c>
       <c r="I42" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J42" s="1">
         <f t="shared" si="2"/>
@@ -2125,7 +2116,7 @@
       </c>
       <c r="K42" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L42" s="1">
         <f t="shared" si="4"/>
@@ -2136,20 +2127,20 @@
       <c r="A43" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3">
-        <v>6.8976499999999996</v>
-      </c>
+      <c r="B43" s="3">
+        <v>17.530999999999999</v>
+      </c>
+      <c r="C43" s="3"/>
       <c r="D43" s="2">
         <v>1</v>
       </c>
       <c r="F43" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="4">
         <f t="shared" si="0"/>
-        <v>6.8976499999999996</v>
+        <v>17.530999999999999</v>
       </c>
       <c r="I43" s="1">
         <f t="shared" si="1"/>
@@ -2161,7 +2152,7 @@
       </c>
       <c r="K43" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L43" s="1">
         <f t="shared" si="4"/>
@@ -2173,27 +2164,23 @@
         <v>53</v>
       </c>
       <c r="B44" s="3">
-        <v>19.733854999999998</v>
-      </c>
-      <c r="C44" s="3">
-        <v>8.9113800000000012</v>
-      </c>
+        <v>32.674809999999994</v>
+      </c>
+      <c r="C44" s="3"/>
       <c r="D44" s="2">
         <v>1</v>
       </c>
       <c r="F44" s="2">
-        <v>2</v>
-      </c>
-      <c r="G44" s="2">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G44" s="2"/>
       <c r="H44" s="4">
         <f t="shared" si="0"/>
-        <v>28.645235</v>
+        <v>32.674809999999994</v>
       </c>
       <c r="I44" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J44" s="1">
         <f t="shared" si="2"/>
@@ -2213,7 +2200,7 @@
         <v>54</v>
       </c>
       <c r="B45" s="3">
-        <v>17.530999999999999</v>
+        <v>32.674809999999994</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="2">
@@ -2225,7 +2212,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="4">
         <f t="shared" si="0"/>
-        <v>17.530999999999999</v>
+        <v>32.674809999999994</v>
       </c>
       <c r="I45" s="1">
         <f t="shared" si="1"/>
@@ -2249,23 +2236,27 @@
         <v>55</v>
       </c>
       <c r="B46" s="3">
-        <v>32.674809999999994</v>
-      </c>
-      <c r="C46" s="3"/>
+        <v>5.1226349999999998</v>
+      </c>
+      <c r="C46" s="3">
+        <v>1.5764499999999999</v>
+      </c>
       <c r="D46" s="2">
         <v>1</v>
       </c>
       <c r="F46" s="2">
-        <v>1</v>
-      </c>
-      <c r="G46" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="G46" s="2">
+        <v>1</v>
+      </c>
       <c r="H46" s="4">
         <f t="shared" si="0"/>
-        <v>32.674809999999994</v>
+        <v>6.6990850000000002</v>
       </c>
       <c r="I46" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J46" s="1">
         <f t="shared" si="2"/>
@@ -2284,20 +2275,20 @@
       <c r="A47" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="3">
-        <v>32.674809999999994</v>
-      </c>
-      <c r="C47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3">
+        <v>1.9446000000000001</v>
+      </c>
       <c r="D47" s="2">
         <v>1</v>
       </c>
       <c r="F47" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="4">
         <f t="shared" si="0"/>
-        <v>32.674809999999994</v>
+        <v>1.9446000000000001</v>
       </c>
       <c r="I47" s="1">
         <f t="shared" si="1"/>
@@ -2309,7 +2300,7 @@
       </c>
       <c r="K47" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L47" s="1">
         <f t="shared" si="4"/>
@@ -2321,31 +2312,25 @@
         <v>57</v>
       </c>
       <c r="B48" s="3">
-        <v>5.1226349999999998</v>
-      </c>
-      <c r="C48" s="3">
-        <v>1.5764499999999999</v>
-      </c>
-      <c r="D48" s="2">
-        <v>1</v>
-      </c>
+        <v>2.1283750000000001</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="2"/>
       <c r="F48" s="2">
-        <v>2</v>
-      </c>
-      <c r="G48" s="2">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G48" s="2"/>
       <c r="H48" s="4">
         <f t="shared" si="0"/>
-        <v>6.6990850000000002</v>
+        <v>2.1283750000000001</v>
       </c>
       <c r="I48" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J48" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K48" s="1">
         <f t="shared" si="3"/>
@@ -2360,28 +2345,30 @@
       <c r="A49" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="3"/>
+      <c r="B49" s="3">
+        <v>8.8796999999999997</v>
+      </c>
       <c r="C49" s="3">
-        <v>1.9446000000000001</v>
-      </c>
-      <c r="D49" s="2">
-        <v>1</v>
-      </c>
+        <v>7.5849000000000002</v>
+      </c>
+      <c r="D49" s="2"/>
       <c r="F49" s="2">
-        <v>2</v>
-      </c>
-      <c r="G49" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="G49" s="2">
+        <v>2</v>
+      </c>
       <c r="H49" s="4">
         <f t="shared" si="0"/>
-        <v>1.9446000000000001</v>
+        <v>16.464600000000001</v>
       </c>
       <c r="I49" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J49" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K49" s="1">
         <f t="shared" si="3"/>
@@ -2389,7 +2376,7 @@
       </c>
       <c r="L49" s="1">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2397,7 +2384,7 @@
         <v>59</v>
       </c>
       <c r="B50" s="3">
-        <v>2.1283750000000001</v>
+        <v>5.4827500000000002</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="2"/>
@@ -2407,7 +2394,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="4">
         <f t="shared" si="0"/>
-        <v>2.1283750000000001</v>
+        <v>5.4827500000000002</v>
       </c>
       <c r="I50" s="1">
         <f t="shared" si="1"/>
@@ -2431,25 +2418,21 @@
         <v>60</v>
       </c>
       <c r="B51" s="3">
-        <v>8.8796999999999997</v>
-      </c>
-      <c r="C51" s="3">
-        <v>7.5849000000000002</v>
-      </c>
+        <v>24.641690000000001</v>
+      </c>
+      <c r="C51" s="3"/>
       <c r="D51" s="2"/>
       <c r="F51" s="2">
         <v>1</v>
       </c>
-      <c r="G51" s="2">
-        <v>2</v>
-      </c>
+      <c r="G51" s="2"/>
       <c r="H51" s="4">
         <f t="shared" si="0"/>
-        <v>16.464600000000001</v>
+        <v>24.641690000000001</v>
       </c>
       <c r="I51" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J51" s="1">
         <f t="shared" si="2"/>
@@ -2457,11 +2440,11 @@
       </c>
       <c r="K51" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L51" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2469,7 +2452,7 @@
         <v>61</v>
       </c>
       <c r="B52" s="3">
-        <v>5.4827500000000002</v>
+        <v>26.595600000000001</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="2"/>
@@ -2479,7 +2462,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="4">
         <f t="shared" si="0"/>
-        <v>5.4827500000000002</v>
+        <v>26.595600000000001</v>
       </c>
       <c r="I52" s="1">
         <f t="shared" si="1"/>
@@ -2503,7 +2486,7 @@
         <v>62</v>
       </c>
       <c r="B53" s="3">
-        <v>24.641690000000001</v>
+        <v>28.8416</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="2"/>
@@ -2513,7 +2496,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="4">
         <f t="shared" si="0"/>
-        <v>24.641690000000001</v>
+        <v>28.8416</v>
       </c>
       <c r="I53" s="1">
         <f t="shared" si="1"/>
@@ -2537,7 +2520,7 @@
         <v>63</v>
       </c>
       <c r="B54" s="3">
-        <v>26.595600000000001</v>
+        <v>26.826000000000001</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="2"/>
@@ -2547,7 +2530,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="4">
         <f t="shared" si="0"/>
-        <v>26.595600000000001</v>
+        <v>26.826000000000001</v>
       </c>
       <c r="I54" s="1">
         <f t="shared" si="1"/>
@@ -2571,7 +2554,7 @@
         <v>64</v>
       </c>
       <c r="B55" s="3">
-        <v>28.8416</v>
+        <v>26.826000000000001</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="2"/>
@@ -2581,7 +2564,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="4">
         <f t="shared" si="0"/>
-        <v>28.8416</v>
+        <v>26.826000000000001</v>
       </c>
       <c r="I55" s="1">
         <f t="shared" si="1"/>
@@ -2605,7 +2588,7 @@
         <v>65</v>
       </c>
       <c r="B56" s="3">
-        <v>26.826000000000001</v>
+        <v>2.7665500000000001</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="2"/>
@@ -2615,7 +2598,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="4">
         <f t="shared" si="0"/>
-        <v>26.826000000000001</v>
+        <v>2.7665500000000001</v>
       </c>
       <c r="I56" s="1">
         <f t="shared" si="1"/>
@@ -2639,7 +2622,7 @@
         <v>66</v>
       </c>
       <c r="B57" s="3">
-        <v>26.826000000000001</v>
+        <v>26.595600000000001</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="2"/>
@@ -2649,7 +2632,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="4">
         <f t="shared" si="0"/>
-        <v>26.826000000000001</v>
+        <v>26.595600000000001</v>
       </c>
       <c r="I57" s="1">
         <f t="shared" si="1"/>
@@ -2672,18 +2655,18 @@
       <c r="A58" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B58" s="3">
-        <v>2.7665500000000001</v>
-      </c>
-      <c r="C58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3">
+        <v>0.97684000000000004</v>
+      </c>
       <c r="D58" s="2"/>
       <c r="F58" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="4">
         <f t="shared" si="0"/>
-        <v>2.7665500000000001</v>
+        <v>0.97684000000000004</v>
       </c>
       <c r="I58" s="1">
         <f t="shared" si="1"/>
@@ -2695,7 +2678,7 @@
       </c>
       <c r="K58" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L58" s="1">
         <f t="shared" si="4"/>
@@ -2707,21 +2690,25 @@
         <v>68</v>
       </c>
       <c r="B59" s="3">
-        <v>26.595600000000001</v>
-      </c>
-      <c r="C59" s="3"/>
+        <v>1.8894500000000001</v>
+      </c>
+      <c r="C59" s="3">
+        <v>0.76963999999999999</v>
+      </c>
       <c r="D59" s="2"/>
       <c r="F59" s="2">
-        <v>1</v>
-      </c>
-      <c r="G59" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="G59" s="2">
+        <v>1</v>
+      </c>
       <c r="H59" s="4">
         <f t="shared" si="0"/>
-        <v>26.595600000000001</v>
+        <v>2.65909</v>
       </c>
       <c r="I59" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J59" s="1">
         <f t="shared" si="2"/>
@@ -2742,7 +2729,7 @@
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3">
-        <v>0.97684000000000004</v>
+        <v>2.9621200000000001</v>
       </c>
       <c r="D60" s="2"/>
       <c r="F60" s="2">
@@ -2751,7 +2738,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="4">
         <f t="shared" si="0"/>
-        <v>0.97684000000000004</v>
+        <v>2.9621200000000001</v>
       </c>
       <c r="I60" s="1">
         <f t="shared" si="1"/>
@@ -2775,21 +2762,21 @@
         <v>70</v>
       </c>
       <c r="B61" s="3">
-        <v>1.8894500000000001</v>
+        <v>11.119145</v>
       </c>
       <c r="C61" s="3">
-        <v>0.76963999999999999</v>
+        <v>9.3242449999999995</v>
       </c>
       <c r="D61" s="2"/>
       <c r="F61" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G61" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H61" s="4">
         <f t="shared" si="0"/>
-        <v>2.65909</v>
+        <v>20.443390000000001</v>
       </c>
       <c r="I61" s="1">
         <f t="shared" si="1"/>
@@ -2801,33 +2788,37 @@
       </c>
       <c r="K61" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L61" s="1">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B62" s="3"/>
+      <c r="B62" s="3">
+        <v>11.119145</v>
+      </c>
       <c r="C62" s="3">
-        <v>2.9621200000000001</v>
+        <v>9.3242449999999995</v>
       </c>
       <c r="D62" s="2"/>
       <c r="F62" s="2">
-        <v>2</v>
-      </c>
-      <c r="G62" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="G62" s="2">
+        <v>2</v>
+      </c>
       <c r="H62" s="4">
         <f t="shared" si="0"/>
-        <v>2.9621200000000001</v>
+        <v>20.443390000000001</v>
       </c>
       <c r="I62" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J62" s="1">
         <f t="shared" si="2"/>
@@ -2839,33 +2830,29 @@
       </c>
       <c r="L62" s="1">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B63" s="3">
-        <v>11.119145</v>
-      </c>
+      <c r="B63" s="3"/>
       <c r="C63" s="3">
-        <v>9.3242449999999995</v>
+        <v>7.7475549999999993</v>
       </c>
       <c r="D63" s="2"/>
       <c r="F63" s="2">
-        <v>1</v>
-      </c>
-      <c r="G63" s="2">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G63" s="2"/>
       <c r="H63" s="4">
         <f t="shared" si="0"/>
-        <v>20.443390000000001</v>
+        <v>7.7475549999999993</v>
       </c>
       <c r="I63" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J63" s="1">
         <f t="shared" si="2"/>
@@ -2877,7 +2864,7 @@
       </c>
       <c r="L63" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2885,10 +2872,10 @@
         <v>73</v>
       </c>
       <c r="B64" s="3">
-        <v>11.119145</v>
+        <v>2.3997299999999999</v>
       </c>
       <c r="C64" s="3">
-        <v>9.3242449999999995</v>
+        <v>4.4859499999999999</v>
       </c>
       <c r="D64" s="2"/>
       <c r="F64" s="2">
@@ -2899,7 +2886,7 @@
       </c>
       <c r="H64" s="4">
         <f t="shared" si="0"/>
-        <v>20.443390000000001</v>
+        <v>6.8856799999999998</v>
       </c>
       <c r="I64" s="1">
         <f t="shared" si="1"/>
@@ -2922,18 +2909,20 @@
       <c r="A65" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3">
-        <v>7.7475549999999993</v>
-      </c>
-      <c r="D65" s="2"/>
+      <c r="B65" s="3">
+        <v>14.928884999999999</v>
+      </c>
+      <c r="C65" s="3"/>
+      <c r="D65" s="2">
+        <v>1</v>
+      </c>
       <c r="F65" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="4">
         <f t="shared" si="0"/>
-        <v>7.7475549999999993</v>
+        <v>14.928884999999999</v>
       </c>
       <c r="I65" s="1">
         <f t="shared" si="1"/>
@@ -2941,11 +2930,11 @@
       </c>
       <c r="J65" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K65" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L65" s="1">
         <f t="shared" si="4"/>
@@ -2957,57 +2946,53 @@
         <v>75</v>
       </c>
       <c r="B66" s="3">
-        <v>2.3997299999999999</v>
-      </c>
-      <c r="C66" s="3">
-        <v>4.4859499999999999</v>
-      </c>
-      <c r="D66" s="2"/>
+        <v>9.4292499999999997</v>
+      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
       <c r="F66" s="2">
         <v>1</v>
       </c>
-      <c r="G66" s="2">
-        <v>2</v>
-      </c>
+      <c r="G66" s="2"/>
       <c r="H66" s="4">
         <f t="shared" si="0"/>
-        <v>6.8856799999999998</v>
+        <v>9.4292499999999997</v>
       </c>
       <c r="I66" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J66" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K66" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L66" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B67" s="3">
-        <v>14.928884999999999</v>
-      </c>
-      <c r="C67" s="3"/>
-      <c r="D67" s="2">
-        <v>1</v>
-      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3">
+        <v>14.712494999999999</v>
+      </c>
+      <c r="D67" s="2"/>
       <c r="F67" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="4">
         <f t="shared" si="0"/>
-        <v>14.928884999999999</v>
+        <v>14.712494999999999</v>
       </c>
       <c r="I67" s="1">
         <f t="shared" si="1"/>
@@ -3015,11 +3000,11 @@
       </c>
       <c r="J67" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K67" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L67" s="1">
         <f t="shared" si="4"/>
@@ -3030,20 +3015,18 @@
       <c r="A68" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B68" s="3">
-        <v>9.4292499999999997</v>
-      </c>
-      <c r="C68" s="3"/>
-      <c r="D68" s="2">
-        <v>1</v>
-      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3">
+        <v>1.9446000000000001</v>
+      </c>
+      <c r="D68" s="2"/>
       <c r="F68" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="4">
         <f t="shared" si="0"/>
-        <v>9.4292499999999997</v>
+        <v>1.9446000000000001</v>
       </c>
       <c r="I68" s="1">
         <f t="shared" si="1"/>
@@ -3051,11 +3034,11 @@
       </c>
       <c r="J68" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K68" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L68" s="1">
         <f t="shared" si="4"/>
@@ -3066,18 +3049,18 @@
       <c r="A69" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3">
-        <v>14.712494999999999</v>
-      </c>
+      <c r="B69" s="3">
+        <v>8.7520000000000007</v>
+      </c>
+      <c r="C69" s="3"/>
       <c r="D69" s="2"/>
       <c r="F69" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="4">
         <f t="shared" si="0"/>
-        <v>14.712494999999999</v>
+        <v>8.7520000000000007</v>
       </c>
       <c r="I69" s="1">
         <f t="shared" si="1"/>
@@ -3089,7 +3072,7 @@
       </c>
       <c r="K69" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L69" s="1">
         <f t="shared" si="4"/>
@@ -3100,18 +3083,18 @@
       <c r="A70" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3">
-        <v>1.9446000000000001</v>
-      </c>
+      <c r="B70" s="3">
+        <v>4.82843</v>
+      </c>
+      <c r="C70" s="3"/>
       <c r="D70" s="2"/>
       <c r="F70" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="4">
         <f t="shared" si="0"/>
-        <v>1.9446000000000001</v>
+        <v>4.82843</v>
       </c>
       <c r="I70" s="1">
         <f t="shared" si="1"/>
@@ -3123,7 +3106,7 @@
       </c>
       <c r="K70" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L70" s="1">
         <f t="shared" si="4"/>
@@ -3135,7 +3118,7 @@
         <v>80</v>
       </c>
       <c r="B71" s="3">
-        <v>8.7520000000000007</v>
+        <v>4.5644499999999999</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="2"/>
@@ -3145,7 +3128,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="4">
         <f t="shared" si="0"/>
-        <v>8.7520000000000007</v>
+        <v>4.5644499999999999</v>
       </c>
       <c r="I71" s="1">
         <f t="shared" si="1"/>
@@ -3169,21 +3152,25 @@
         <v>81</v>
       </c>
       <c r="B72" s="3">
-        <v>4.82843</v>
-      </c>
-      <c r="C72" s="3"/>
+        <v>1.5787599999999999</v>
+      </c>
+      <c r="C72" s="3">
+        <v>15.547134999999999</v>
+      </c>
       <c r="D72" s="2"/>
       <c r="F72" s="2">
-        <v>1</v>
-      </c>
-      <c r="G72" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="G72" s="2">
+        <v>1</v>
+      </c>
       <c r="H72" s="4">
         <f t="shared" si="0"/>
-        <v>4.82843</v>
+        <v>17.125895</v>
       </c>
       <c r="I72" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J72" s="1">
         <f t="shared" si="2"/>
@@ -3203,7 +3190,7 @@
         <v>82</v>
       </c>
       <c r="B73" s="3">
-        <v>4.5644499999999999</v>
+        <v>2.1283750000000001</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="2"/>
@@ -3213,7 +3200,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="4">
         <f t="shared" si="0"/>
-        <v>4.5644499999999999</v>
+        <v>2.1283750000000001</v>
       </c>
       <c r="I73" s="1">
         <f t="shared" si="1"/>
@@ -3237,25 +3224,21 @@
         <v>83</v>
       </c>
       <c r="B74" s="3">
-        <v>1.5787599999999999</v>
-      </c>
-      <c r="C74" s="3">
-        <v>15.547134999999999</v>
-      </c>
+        <v>0.93293000000000004</v>
+      </c>
+      <c r="C74" s="3"/>
       <c r="D74" s="2"/>
       <c r="F74" s="2">
-        <v>2</v>
-      </c>
-      <c r="G74" s="2">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G74" s="2"/>
       <c r="H74" s="4">
         <f t="shared" si="0"/>
-        <v>17.125895</v>
+        <v>0.93293000000000004</v>
       </c>
       <c r="I74" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J74" s="1">
         <f t="shared" si="2"/>
@@ -3275,7 +3258,7 @@
         <v>84</v>
       </c>
       <c r="B75" s="3">
-        <v>2.1283750000000001</v>
+        <v>1.8118000000000001</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="2"/>
@@ -3285,7 +3268,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="4">
         <f t="shared" si="0"/>
-        <v>2.1283750000000001</v>
+        <v>1.8118000000000001</v>
       </c>
       <c r="I75" s="1">
         <f t="shared" si="1"/>
@@ -3309,7 +3292,7 @@
         <v>85</v>
       </c>
       <c r="B76" s="3">
-        <v>0.93293000000000004</v>
+        <v>1.8118000000000001</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="2"/>
@@ -3319,7 +3302,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="4">
         <f t="shared" si="0"/>
-        <v>0.93293000000000004</v>
+        <v>1.8118000000000001</v>
       </c>
       <c r="I76" s="1">
         <f t="shared" si="1"/>
@@ -3343,33 +3326,39 @@
         <v>86</v>
       </c>
       <c r="B77" s="3">
-        <v>1.8118000000000001</v>
-      </c>
-      <c r="C77" s="3"/>
-      <c r="D77" s="2"/>
+        <v>6.9123549999999998</v>
+      </c>
+      <c r="C77" s="3">
+        <v>5.79</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
       <c r="F77" s="2">
         <v>1</v>
       </c>
-      <c r="G77" s="2"/>
+      <c r="G77" s="2">
+        <v>2</v>
+      </c>
       <c r="H77" s="4">
         <f t="shared" si="0"/>
-        <v>1.8118000000000001</v>
+        <v>12.702355000000001</v>
       </c>
       <c r="I77" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J77" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K77" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L77" s="1">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3377,114 +3366,48 @@
         <v>87</v>
       </c>
       <c r="B78" s="3">
-        <v>1.8118000000000001</v>
-      </c>
-      <c r="C78" s="3"/>
-      <c r="D78" s="2"/>
+        <v>6.9123549999999998</v>
+      </c>
+      <c r="C78" s="3">
+        <v>5.79</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
       <c r="F78" s="2">
         <v>1</v>
       </c>
-      <c r="G78" s="2"/>
+      <c r="G78" s="2">
+        <v>2</v>
+      </c>
       <c r="H78" s="4">
         <f t="shared" si="0"/>
-        <v>1.8118000000000001</v>
+        <v>12.702355000000001</v>
       </c>
       <c r="I78" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J78" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K78" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L78" s="1">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B79" s="3">
-        <v>6.9123549999999998</v>
-      </c>
-      <c r="C79" s="3">
-        <v>5.79</v>
-      </c>
-      <c r="D79" s="2">
-        <v>1</v>
-      </c>
-      <c r="F79" s="2">
-        <v>1</v>
-      </c>
-      <c r="G79" s="2">
-        <v>2</v>
-      </c>
-      <c r="H79" s="4">
-        <f t="shared" si="0"/>
-        <v>12.702355000000001</v>
-      </c>
-      <c r="I79" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="J79" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K79" s="1">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L79" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
     </row>
     <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B80" s="3">
-        <v>6.9123549999999998</v>
-      </c>
-      <c r="C80" s="3">
-        <v>5.79</v>
-      </c>
-      <c r="D80" s="2">
-        <v>1</v>
-      </c>
-      <c r="F80" s="2">
-        <v>1</v>
-      </c>
-      <c r="G80" s="2">
-        <v>2</v>
-      </c>
-      <c r="H80" s="4">
-        <f t="shared" si="0"/>
-        <v>12.702355000000001</v>
-      </c>
-      <c r="I80" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="J80" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K80" s="1">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L80" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
     </row>
     <row r="81" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F81" s="2"/>
@@ -7150,15 +7073,8 @@
       <c r="F996" s="2"/>
       <c r="G996" s="2"/>
     </row>
-    <row r="997" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F997" s="2"/>
-      <c r="G997" s="2"/>
-    </row>
-    <row r="998" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F998" s="2"/>
-      <c r="G998" s="2"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:L78" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>